<commit_message>
Modified: Reading and Writing from File
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/xlsxfiles/FacebookTestData.xlsx
+++ b/DataDrivenFramework/xlsxfiles/FacebookTestData.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">john@123456</t>
   </si>
   <si>
-    <t xml:space="preserve">15/Aug/1969</t>
+    <t xml:space="preserve">15/Aug/1968</t>
   </si>
   <si>
     <t xml:space="preserve">Mayuresh</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Sonar</t>
   </si>
   <si>
-    <t xml:space="preserve">Mayuresh@gmail.com</t>
+    <t xml:space="preserve">mayuresh@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Mayur@123456</t>
@@ -76,13 +76,13 @@
     <t xml:space="preserve">Agarwal</t>
   </si>
   <si>
-    <t xml:space="preserve">Ankush@gmail.com</t>
+    <t xml:space="preserve">ankush@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ankush@123456</t>
   </si>
   <si>
-    <t xml:space="preserve">19/Dec/1997</t>
+    <t xml:space="preserve">23/Dec/1997</t>
   </si>
   <si>
     <t xml:space="preserve">Rohit</t>
@@ -91,13 +91,13 @@
     <t xml:space="preserve">Thorawade</t>
   </si>
   <si>
-    <t xml:space="preserve">Rohit@gmail.com</t>
+    <t xml:space="preserve">rohit@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Rohit@123456</t>
   </si>
   <si>
-    <t xml:space="preserve">1/Jul/1996</t>
+    <t xml:space="preserve">12/Jul/1995</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,13 +136,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -216,15 +209,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,7 +225,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,19 +306,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,9 +338,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -433,14 +428,14 @@
     <hyperlink ref="C2" r:id="rId1" display="john@gmail.com"/>
     <hyperlink ref="D2" r:id="rId2" display="john@gmail.com"/>
     <hyperlink ref="E2" r:id="rId3" display="john@123456"/>
-    <hyperlink ref="C3" r:id="rId4" display="Mayuresh@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId5" display="Mayuresh@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId4" display="mayuresh@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId5" display="mayuresh@gmail.com"/>
     <hyperlink ref="E3" r:id="rId6" display="Mayur@123456"/>
-    <hyperlink ref="C4" r:id="rId7" display="Ankush@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId8" display="Ankush@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId7" display="ankush@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId8" display="ankush@gmail.com"/>
     <hyperlink ref="E4" r:id="rId9" display="Ankush@123456"/>
-    <hyperlink ref="C5" r:id="rId10" display="Rohit@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId11" display="Rohit@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId10" display="rohit@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId11" display="rohit@gmail.com"/>
     <hyperlink ref="E5" r:id="rId12" display="Rohit@123456"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Modified: Facebook Login Test using Data Provider
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/xlsxfiles/FacebookTestData.xlsx
+++ b/DataDrivenFramework/xlsxfiles/FacebookTestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegDataTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="LoginDataTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -40,6 +41,9 @@
     <t xml:space="preserve">Birthday</t>
   </si>
   <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
@@ -55,6 +59,9 @@
     <t xml:space="preserve">15/Aug/1968</t>
   </si>
   <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mayuresh</t>
   </si>
   <si>
@@ -98,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">12/Jul/1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userName</t>
   </si>
 </sst>
 </file>
@@ -107,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,8 +154,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,7 +172,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8AA97"/>
-        <bgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFF7A19A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7A19A"/>
+        <bgColor rgb="FFF8AA97"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,6 +232,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,6 +250,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -273,9 +308,9 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFF7A19A"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8AA97"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -302,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,7 +348,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,85 +372,100 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -439,4 +491,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mayuresh@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Mayur@123456"/>
+    <hyperlink ref="A3" r:id="rId3" display="ankush@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId4" display="Ankush@123456"/>
+    <hyperlink ref="A4" r:id="rId5" display="rohit@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId6" display="Rohit@123456"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>